<commit_message>
fix 131_1_20 to 131_0_20
</commit_message>
<xml_diff>
--- a/Used-Journal-Subjective_Eval/文件名_new.xlsx
+++ b/Used-Journal-Subjective_Eval/文件名_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hui Lu\Desktop\luhui\projects\xx_mos_files\Used-Journal-Subjective_Eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F52FCFB-31D8-465E-A61D-0F8B55357A86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84324D2E-BAF2-4B03-9285-EAAC24435349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>parallel-MOS TEST1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -246,6 +246,26 @@
   </si>
   <si>
     <t>1 4 3 2 5</t>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -608,7 +628,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
@@ -617,303 +637,363 @@
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.234375" customWidth="1"/>
-    <col min="2" max="2" width="9.29296875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.1171875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="38.76171875" customWidth="1"/>
-    <col min="5" max="5" width="33.8203125" customWidth="1"/>
+    <col min="2" max="3" width="9.29296875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.1171875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="38.76171875" customWidth="1"/>
+    <col min="6" max="6" width="33.8203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4">
         <v>32</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4">
         <v>7</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4">
         <v>10</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="4">
         <v>11</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="4">
         <v>8</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="4">
         <v>13</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="4">
         <v>15</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="4">
         <v>17</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="4">
         <v>20</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="4">
         <v>19</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="4">
         <v>34</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="4">
         <v>23</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="4">
         <v>24</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="4">
         <v>39</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="4">
         <v>41</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="4">
         <v>28</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="4">
         <v>31</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add mos analysis script
</commit_message>
<xml_diff>
--- a/Used-Journal-Subjective_Eval/文件名_new.xlsx
+++ b/Used-Journal-Subjective_Eval/文件名_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hui Lu\Desktop\luhui\projects\xx_mos_files\Used-Journal-Subjective_Eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D81A0D8-D455-4FBA-BD6C-68855CF5A9C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32A8869-32EB-4581-ACB9-F1B497152B71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="13520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -319,9 +319,6 @@
     <t>AMidsummerNightsDream--145_0_t15</t>
   </si>
   <si>
-    <t>AMidsummerNightsDream--410_t17</t>
-  </si>
-  <si>
     <t>AMidsummerNightsDream--189_t21</t>
   </si>
   <si>
@@ -364,6 +361,10 @@
   </si>
   <si>
     <t>AMidsummerNightsDream--368_t25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMidsummerNightsDream--410_t22</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -739,7 +740,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
@@ -1336,7 +1337,7 @@
         <v>51</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
@@ -1356,7 +1357,7 @@
         <v>52</v>
       </c>
       <c r="F33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
@@ -1376,7 +1377,7 @@
         <v>53</v>
       </c>
       <c r="F34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
@@ -1390,13 +1391,13 @@
         <v>17</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
@@ -1416,7 +1417,7 @@
         <v>55</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
@@ -1430,13 +1431,13 @@
         <v>19</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>56</v>
       </c>
       <c r="F37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -1450,13 +1451,13 @@
         <v>34</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
@@ -1476,7 +1477,7 @@
         <v>58</v>
       </c>
       <c r="F39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
@@ -1490,13 +1491,13 @@
         <v>24</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
@@ -1516,7 +1517,7 @@
         <v>60</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
@@ -1524,7 +1525,7 @@
         <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C42" s="3">
         <v>41</v>
@@ -1536,7 +1537,7 @@
         <v>61</v>
       </c>
       <c r="F42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
@@ -1556,7 +1557,7 @@
         <v>62</v>
       </c>
       <c r="F43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
@@ -1576,12 +1577,12 @@
         <v>63</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>